<commit_message>
Automation of valid login tc
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adity\Desktop\TRI_DOCUMENTS\1PYTHON and SELENIUM\Selenium recordings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adity\PycharmProjects\B105AFWW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EB8007-CDFF-4A37-87B8-96F78B14EC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE541DF4-F324-4C3C-8D21-A1C88B83EAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tc1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -357,7 +357,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>